<commit_message>
+ task input from
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -9,14 +9,14 @@
   <sheets>
     <sheet name="crtTask" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="taskInput" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="95">
   <si>
     <t>#task - cong viec</t>
   </si>
@@ -250,6 +250,57 @@
   </si>
   <si>
     <t>end_date</t>
+  </si>
+  <si>
+    <t>#dbschema</t>
+  </si>
+  <si>
+    <t>#inputPanel</t>
+  </si>
+  <si>
+    <t>taskInputPanel</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>dict</t>
+  </si>
+  <si>
+    <t>#menu</t>
+  </si>
+  <si>
+    <t>#inputF</t>
+  </si>
+  <si>
+    <t>lTaskInputF</t>
+  </si>
+  <si>
+    <t>miInput</t>
+  </si>
+  <si>
+    <t>miTask</t>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>order_number</t>
+  </si>
+  <si>
+    <t>task-order</t>
+  </si>
+  <si>
+    <t>lOrderInpuF</t>
   </si>
 </sst>
 </file>
@@ -305,7 +356,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -313,11 +364,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -330,6 +461,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="F16" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,10 +1409,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,6 +1474,82 @@
       <c r="B9" t="s">
         <v>71</v>
       </c>
+      <c r="E9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1343,12 +1558,160 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="14"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="15"/>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="15"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="14"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="15"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="14"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="15"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="14"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="15"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="14"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="15"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="14"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="15"/>
+      <c r="I8" s="15"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="14"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="15"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="14"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="15"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="14"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="15"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="14"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="15"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="14"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="15"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="18"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
res; orderRes; custom dgv
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="crtTask" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="taskInput" sheetId="3" r:id="rId3"/>
+    <sheet name="taskInput" sheetId="3" r:id="rId2"/>
+    <sheet name="orderInput" sheetId="4" r:id="rId3"/>
+    <sheet name="res" sheetId="5" r:id="rId4"/>
+    <sheet name="search" sheetId="6" r:id="rId5"/>
+    <sheet name="NOTE" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="198">
   <si>
     <t>#task - cong viec</t>
   </si>
@@ -117,9 +120,6 @@
     <t>number</t>
   </si>
   <si>
-    <t>comment</t>
-  </si>
-  <si>
     <t>requesting</t>
   </si>
   <si>
@@ -297,10 +297,322 @@
     <t>order_number</t>
   </si>
   <si>
-    <t>task-order</t>
-  </si>
-  <si>
     <t>lOrderInpuF</t>
+  </si>
+  <si>
+    <t>order_type</t>
+  </si>
+  <si>
+    <t>(số lượng)</t>
+  </si>
+  <si>
+    <t>(ghi chú)</t>
+  </si>
+  <si>
+    <t>lOrderDataPanel</t>
+  </si>
+  <si>
+    <t>order_status</t>
+  </si>
+  <si>
+    <t>lOrderSearchPanel</t>
+  </si>
+  <si>
+    <t>lOrderPanel</t>
+  </si>
+  <si>
+    <t>lOrderReport</t>
+  </si>
+  <si>
+    <t>#lDataSync</t>
+  </si>
+  <si>
+    <t>Refresh()</t>
+  </si>
+  <si>
+    <t>col[1]</t>
+  </si>
+  <si>
+    <t>zero base</t>
+  </si>
+  <si>
+    <t>lOrderTblInfo</t>
+  </si>
+  <si>
+    <t>order_tbl</t>
+  </si>
+  <si>
+    <t>#form1</t>
+  </si>
+  <si>
+    <t>appConfig.s_config.m_panels</t>
+  </si>
+  <si>
+    <t>miOrder</t>
+  </si>
+  <si>
+    <t>lAdvanceStatus</t>
+  </si>
+  <si>
+    <t>lOrderStatus</t>
+  </si>
+  <si>
+    <t>(đang xin phép)</t>
+  </si>
+  <si>
+    <t>( đã chấp nhận)</t>
+  </si>
+  <si>
+    <t>order-status</t>
+  </si>
+  <si>
+    <t>status - col type map</t>
+  </si>
+  <si>
+    <t>resource list</t>
+  </si>
+  <si>
+    <t>res_xxx</t>
+  </si>
+  <si>
+    <t>res_yyy</t>
+  </si>
+  <si>
+    <t>order-resource</t>
+  </si>
+  <si>
+    <t>order_xxx_1</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>nhan su</t>
+  </si>
+  <si>
+    <t>cong viec</t>
+  </si>
+  <si>
+    <t>cv_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>down</t>
+  </si>
+  <si>
+    <t>up</t>
+  </si>
+  <si>
+    <t>#human</t>
+  </si>
+  <si>
+    <t>human_id</t>
+  </si>
+  <si>
+    <t>#equipment</t>
+  </si>
+  <si>
+    <t>ordertype change</t>
+  </si>
+  <si>
+    <t>EditingCompleted</t>
+  </si>
+  <si>
+    <t>data content</t>
+  </si>
+  <si>
+    <t>lDataContent dc = appConfig.s_contentProvider.CreateDataContent("human");</t>
+  </si>
+  <si>
+    <t>human_number</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>(0:nam,1 nu)</t>
+  </si>
+  <si>
+    <t>human</t>
+  </si>
+  <si>
+    <t>equipment</t>
+  </si>
+  <si>
+    <t>lEquipmentDataPanel</t>
+  </si>
+  <si>
+    <t>lHumanDataPanel</t>
+  </si>
+  <si>
+    <t>lEquipmentSearchPanel</t>
+  </si>
+  <si>
+    <t>lHumanSearchPanel</t>
+  </si>
+  <si>
+    <t>lEquipmentReport</t>
+  </si>
+  <si>
+    <t>lHumanReport</t>
+  </si>
+  <si>
+    <t>lHumanPanel</t>
+  </si>
+  <si>
+    <t>lEquipmentPanel</t>
+  </si>
+  <si>
+    <t>lHumanTblInfo</t>
+  </si>
+  <si>
+    <t>lEquipmentTblInfo</t>
+  </si>
+  <si>
+    <t>lOrderType</t>
+  </si>
+  <si>
+    <t>lConfigMng.parseEnum</t>
+  </si>
+  <si>
+    <t>lApproveInputF</t>
+  </si>
+  <si>
+    <t>lApproveInputPanel</t>
+  </si>
+  <si>
+    <t>miApprove</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>remain</t>
+  </si>
+  <si>
+    <t>nếu số lượng thiết bị request &gt; số thiết bị hiện có</t>
+  </si>
+  <si>
+    <t>"=&gt;reject yêu cẩu?</t>
+  </si>
+  <si>
+    <t>ban quản lý mua thêm và approve?</t>
+  </si>
+  <si>
+    <t>tổng số</t>
+  </si>
+  <si>
+    <t>số lượng còn lại</t>
+  </si>
+  <si>
+    <t>tìm kiếm công việc đã approve</t>
+  </si>
+  <si>
+    <t>ngay vao</t>
+  </si>
+  <si>
+    <t>ngay ra</t>
+  </si>
+  <si>
+    <t>search cu si o chua tu ngay xxx toi yyy</t>
+  </si>
+  <si>
+    <t>ngay vao = xxx and ngay ra = yyy</t>
+  </si>
+  <si>
+    <t>search cu si vao chua tu ngay xxx</t>
+  </si>
+  <si>
+    <t>ngay vao &gt;= xxx</t>
+  </si>
+  <si>
+    <t>search cu si o chua toi ngay yyy</t>
+  </si>
+  <si>
+    <t>ngay ra &gt;= yyy</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>(còn lại)</t>
+  </si>
+  <si>
+    <t>công việc có order bị reject -&gt;cần sửa lại yêu cầu?</t>
+  </si>
+  <si>
+    <t>mã CV</t>
+  </si>
+  <si>
+    <t>(tự sinh)</t>
+  </si>
+  <si>
+    <t>thuộc ban</t>
+  </si>
+  <si>
+    <t>nội dung</t>
+  </si>
+  <si>
+    <t>ngày bắt đầu</t>
+  </si>
+  <si>
+    <t>ngày kết thúc</t>
+  </si>
+  <si>
+    <t>ghi chú</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>tìm nhân sự cho công việc</t>
+  </si>
+  <si>
+    <t>tìm thiết bị cho công việc (vd: công việc cần lọai ô tô tải)</t>
+  </si>
+  <si>
+    <t>loại TB</t>
+  </si>
+  <si>
+    <t>Ô tô tải</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>(biển số)</t>
+  </si>
+  <si>
+    <t>#car</t>
+  </si>
+  <si>
+    <t>(4 chỗ, 8 chỗ)</t>
+  </si>
+  <si>
+    <t>toyota</t>
+  </si>
+  <si>
+    <t>car_number</t>
+  </si>
+  <si>
+    <t>car_type</t>
+  </si>
+  <si>
+    <t>CarTblInfo</t>
+  </si>
+  <si>
+    <t>#order_car(1-n)</t>
   </si>
 </sst>
 </file>
@@ -324,7 +636,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,8 +667,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -444,11 +774,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -469,6 +851,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,6 +886,208 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>400049</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangular Callout 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6315074" y="38099"/>
+          <a:ext cx="1400175" cy="752475"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -72534"/>
+            <a:gd name="adj2" fmla="val 37803"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>update "resource list" by "order_type"</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangular Callout 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1924050" y="2457450"/>
+          <a:ext cx="1400175" cy="752475"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -44643"/>
+            <a:gd name="adj2" fmla="val -110298"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>when delete order</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> -&gt;delete relate order-resource records</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangular Callout 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6324600" y="1466850"/>
+          <a:ext cx="1800225" cy="857250"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -73895"/>
+            <a:gd name="adj2" fmla="val -77387"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>"down":</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> add resource to order</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>"up": release resource from order</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -770,16 +1377,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView topLeftCell="F16" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.5703125" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
@@ -787,19 +1394,20 @@
     <col min="10" max="10" width="18" customWidth="1"/>
     <col min="11" max="11" width="19.7109375" customWidth="1"/>
     <col min="12" max="12" width="11.85546875" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -807,10 +1415,10 @@
         <v>13</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -818,10 +1426,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -830,7 +1438,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -841,10 +1449,10 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -853,7 +1461,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -864,10 +1472,10 @@
         <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H5">
         <v>3</v>
@@ -876,7 +1484,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -887,7 +1495,7 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H6">
         <v>4</v>
@@ -896,7 +1504,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -907,7 +1515,7 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H7">
         <v>5</v>
@@ -916,7 +1524,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -927,22 +1535,22 @@
         <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>24</v>
       </c>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I9" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
@@ -965,13 +1573,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
       <c r="I11" s="2" t="s">
         <v>27</v>
       </c>
@@ -991,24 +1596,30 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>72</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>91</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>7</v>
@@ -1017,7 +1628,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1027,6 +1638,9 @@
       <c r="D14" t="s">
         <v>12</v>
       </c>
+      <c r="F14" t="s">
+        <v>97</v>
+      </c>
       <c r="I14" s="5" t="s">
         <v>8</v>
       </c>
@@ -1040,10 +1654,13 @@
         <v>10</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I15" s="2">
         <v>1</v>
       </c>
@@ -1054,15 +1671,24 @@
         <v>28</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="F16" t="s">
+        <v>106</v>
       </c>
       <c r="I16">
         <v>2</v>
@@ -1071,22 +1697,31 @@
         <v>27</v>
       </c>
       <c r="K16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L16" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="M16" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <v>2</v>
+      </c>
+      <c r="R16" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
+      <c r="F17" t="s">
+        <v>91</v>
+      </c>
       <c r="I17">
         <v>3</v>
       </c>
@@ -1094,16 +1729,19 @@
         <v>27</v>
       </c>
       <c r="K17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="L17" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R17" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1113,17 +1751,26 @@
       <c r="D18" t="s">
         <v>31</v>
       </c>
+      <c r="F18" t="s">
+        <v>93</v>
+      </c>
       <c r="I18" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="P18" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
       </c>
+      <c r="D19" t="s">
+        <v>94</v>
+      </c>
       <c r="I19" s="5" t="s">
         <v>9</v>
       </c>
@@ -1134,71 +1781,101 @@
         <v>32</v>
       </c>
       <c r="L19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R19" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
+      <c r="D20" t="s">
+        <v>95</v>
+      </c>
       <c r="I20" s="2" t="s">
         <v>28</v>
       </c>
       <c r="J20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K20">
         <v>1</v>
       </c>
       <c r="L20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="R20" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K21">
         <v>1</v>
       </c>
       <c r="L21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>129</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
+      <c r="F23" t="s">
+        <v>135</v>
+      </c>
       <c r="H23" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>16</v>
+      </c>
       <c r="I24" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>136</v>
+      </c>
+      <c r="F25" t="s">
+        <v>75</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>8</v>
@@ -1207,43 +1884,45 @@
         <v>9</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" t="s">
-        <v>2</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>139</v>
+      </c>
+      <c r="F26" t="s">
+        <v>76</v>
       </c>
       <c r="I26">
         <v>1</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F28" s="2"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F28" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="I28" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" t="s">
-        <v>2</v>
-      </c>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="2"/>
       <c r="I29" s="5" t="s">
         <v>8</v>
       </c>
@@ -1251,15 +1930,12 @@
         <v>9</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" t="s">
-        <v>2</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2">
@@ -1269,36 +1945,34 @@
         <v>28</v>
       </c>
       <c r="K30" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C31" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I32" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -1312,10 +1986,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -1343,6 +2014,8 @@
       <c r="C35" t="s">
         <v>2</v>
       </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2">
         <v>1</v>
@@ -1354,15 +2027,15 @@
         <v>28</v>
       </c>
       <c r="L35" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
@@ -1375,13 +2048,13 @@
         <v>27</v>
       </c>
       <c r="K36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L36" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="M36" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="L36" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="M36" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -1392,13 +2065,140 @@
         <v>27</v>
       </c>
       <c r="K37" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L37" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M37" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="L37" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="M37" s="6" t="s">
-        <v>59</v>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>157</v>
+      </c>
+      <c r="D46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>158</v>
+      </c>
+      <c r="D47" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>190</v>
+      </c>
+      <c r="F50" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>192</v>
+      </c>
+      <c r="F51" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>189</v>
+      </c>
+      <c r="C52" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" t="s">
+        <v>193</v>
+      </c>
+      <c r="F52" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -1409,147 +2209,122 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="B2:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" customWidth="1"/>
-    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>84</v>
-      </c>
-      <c r="E16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>94</v>
-      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="14"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="15"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="E4" s="38"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="22"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="22"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="22"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" s="21"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="22"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="C9" s="21"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="22"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="14"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="14"/>
+      <c r="C11" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="20"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="14"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="14"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1558,158 +2333,894 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I14"/>
+  <dimension ref="A2:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="19" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="38"/>
+      <c r="G4" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="25"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G5" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="31"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G6" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="15"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="13"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="14"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="15"/>
-      <c r="F3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="14"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="15"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="14"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="15"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="14"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="2"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="15"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="14"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="15"/>
-      <c r="I8" s="15"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>91</v>
-      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="15"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G8" s="16"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="15"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="14"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="15"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="15"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I9" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="J9" s="36" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="G10" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="35"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="28"/>
+      <c r="G11" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="15"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="2"/>
+      <c r="G12" s="14"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="15"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I12" s="2"/>
+      <c r="J12" s="15"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="15"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="2"/>
+      <c r="G13" s="14"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="15"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="18"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="15"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="14"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="15"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="14"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="15"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="15"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="18"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="18"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G22" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="I22" s="39"/>
+      <c r="J22" s="42" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" s="35"/>
+      <c r="D24" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" s="38"/>
+      <c r="G24" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="25"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G25" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="31"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G26" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="15"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="35"/>
+      <c r="D27" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" s="22"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="15"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G28" s="16"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="18"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="J29" s="36" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="G30" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="35"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" s="28"/>
+      <c r="G31" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J31" s="13"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="14"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="15"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="15"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="14"/>
+      <c r="C33" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="15"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="15"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="14"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="15"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="15"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="14"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="15"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="15"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="16"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="18"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J58"/>
+  <sheetViews>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>145</v>
+      </c>
+      <c r="E13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>142</v>
+      </c>
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" t="s">
+        <v>152</v>
+      </c>
+      <c r="G22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>140</v>
+      </c>
+      <c r="E24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>141</v>
+      </c>
+      <c r="E26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>196</v>
+      </c>
+      <c r="E28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>196</v>
+      </c>
+      <c r="E38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>79</v>
+      </c>
+      <c r="E43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>83</v>
+      </c>
+      <c r="E47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>87</v>
+      </c>
+      <c r="E48" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>109</v>
+      </c>
+      <c r="E49" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>85</v>
+      </c>
+      <c r="E52" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>92</v>
+      </c>
+      <c r="E53" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>111</v>
+      </c>
+      <c r="F54" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>131</v>
+      </c>
+      <c r="F55" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>133</v>
+      </c>
+      <c r="F56" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>155</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>